<commit_message>
Add booking date in invoice annexure before closed date #CRM-391
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ANNEXURE - INSTALLATION &amp; DEMO</t>
   </si>
@@ -91,6 +91,9 @@
     <t>247Around Item ID</t>
   </si>
   <si>
+    <t>Booking Date</t>
+  </si>
+  <si>
     <t>Closed Date</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
   </si>
   <si>
     <t>{booking:unit_id}</t>
+  </si>
+  <si>
+    <t>{booking:booking_date}</t>
   </si>
   <si>
     <t>{booking:closed_date}</t>
@@ -291,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -353,10 +359,16 @@
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="6" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -396,9 +408,9 @@
     <col customWidth="1" min="9" max="9" width="19.86"/>
     <col customWidth="1" min="10" max="10" width="14.43"/>
     <col customWidth="1" min="11" max="12" width="23.29"/>
-    <col customWidth="1" min="13" max="13" width="18.71"/>
-    <col customWidth="1" min="14" max="14" width="22.0"/>
-    <col customWidth="1" min="15" max="17" width="14.43"/>
+    <col customWidth="1" min="13" max="14" width="18.71"/>
+    <col customWidth="1" min="15" max="15" width="22.0"/>
+    <col customWidth="1" min="16" max="18" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -418,6 +430,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -437,8 +450,9 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="5"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -457,7 +471,8 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="7"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -478,7 +493,8 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="7"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
@@ -493,15 +509,15 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="K5" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="1"/>
+      <c r="M5" s="11"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="7"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -516,15 +532,15 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" s="1"/>
+      <c r="M6" s="11"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="7"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
@@ -539,15 +555,15 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7" s="1"/>
+      <c r="M7" s="11"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="7"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -563,10 +579,10 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="7"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -582,10 +598,10 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="7"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
@@ -600,15 +616,15 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="K10" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="N10" s="16"/>
-      <c r="O10" s="1"/>
+      <c r="M10" s="15"/>
+      <c r="O10" s="16"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="7"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
@@ -623,30 +639,30 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="1"/>
+      <c r="M11" s="11"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="7"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="L12" s="16"/>
-      <c r="M12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="16"/>
-      <c r="O12" s="1"/>
+      <c r="M12" s="15"/>
+      <c r="O12" s="16"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="7"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
@@ -655,9 +671,10 @@
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
-      <c r="O13" s="1"/>
+      <c r="O13" s="16"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="7"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
@@ -676,9 +693,10 @@
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
-      <c r="O14" s="1"/>
+      <c r="O14" s="16"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="7"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
@@ -695,9 +713,10 @@
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
-      <c r="O15" s="1"/>
+      <c r="O15" s="16"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="7"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
@@ -734,7 +753,7 @@
       <c r="L16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="23" t="s">
         <v>26</v>
       </c>
       <c r="N16" s="22" t="s">
@@ -746,79 +765,86 @@
       <c r="P16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="23" t="s">
+      <c r="Q16" s="22" t="s">
         <v>30</v>
+      </c>
+      <c r="R16" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="24" t="s">
         <v>32</v>
       </c>
+      <c r="C17" s="25" t="s">
+        <v>33</v>
+      </c>
       <c r="D17" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="11" t="s">
         <v>42</v>
       </c>
+      <c r="M17" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="N17" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q17" s="25" t="s">
         <v>46</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R17" s="27" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="30"/>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
@@ -826,7 +852,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B12:J13"/>
-    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B2:P2"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Serial No Check Improvement #CRM-756
1. If serial number is not as per the configured format and SF is not
able to complete booking, SF should be able to upload serial number
picture and mark that booking as Completed.
2. This serial number picture link should go in our Invoice Annexure to
Partner so that he can verify this serial number.
3. This serial number picture is visible on all CRMs.
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>ANNEXURE - INSTALLATION &amp; DEMO</t>
   </si>
@@ -67,6 +67,9 @@
     <t>Serial Number</t>
   </si>
   <si>
+    <t>Serial Number Imag</t>
+  </si>
+  <si>
     <t>Customer Name</t>
   </si>
   <si>
@@ -116,6 +119,9 @@
   </si>
   <si>
     <t>{booking:serial_number}</t>
+  </si>
+  <si>
+    <t>{booking:serial_number_pic}</t>
   </si>
   <si>
     <t>{booking:name}</t>
@@ -234,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="14">
     <border/>
     <border>
       <left style="medium">
@@ -291,23 +297,6 @@
       <top/>
     </border>
     <border>
-      <right/>
-      <top/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <bottom/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -344,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -373,6 +362,9 @@
     <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -397,14 +389,14 @@
     <xf borderId="6" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="8" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -417,28 +409,34 @@
     <xf borderId="7" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="7" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="7" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -466,15 +464,15 @@
     <col customWidth="1" min="1" max="1" width="2.14"/>
     <col customWidth="1" min="2" max="2" width="14.14"/>
     <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="5" width="18.57"/>
-    <col customWidth="1" min="6" max="8" width="14.14"/>
-    <col customWidth="1" min="9" max="9" width="19.57"/>
-    <col customWidth="1" min="10" max="10" width="14.14"/>
-    <col customWidth="1" min="11" max="12" width="23.0"/>
-    <col customWidth="1" min="13" max="14" width="18.43"/>
-    <col customWidth="1" min="15" max="15" width="21.71"/>
-    <col customWidth="1" min="16" max="18" width="14.14"/>
-    <col customWidth="1" min="19" max="26" width="8.71"/>
+    <col customWidth="1" min="4" max="6" width="18.57"/>
+    <col customWidth="1" min="7" max="9" width="14.14"/>
+    <col customWidth="1" min="10" max="10" width="19.57"/>
+    <col customWidth="1" min="11" max="11" width="14.14"/>
+    <col customWidth="1" min="12" max="13" width="23.0"/>
+    <col customWidth="1" min="14" max="15" width="18.43"/>
+    <col customWidth="1" min="16" max="16" width="21.71"/>
+    <col customWidth="1" min="17" max="19" width="14.14"/>
+    <col customWidth="1" min="20" max="27" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -495,6 +493,7 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -515,8 +514,9 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="5"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -536,7 +536,8 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="7"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -545,7 +546,7 @@
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -558,373 +559,383 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="7"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="1"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="11"/>
-      <c r="O5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="12"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="7"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="1"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="1"/>
+      <c r="L6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="11"/>
-      <c r="O6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="12"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="7"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="1"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="1"/>
+      <c r="L7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="11"/>
-      <c r="O7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="12"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="7"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="6"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="N8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="7"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="6"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="N9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="7"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="15" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="15"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="16"/>
+      <c r="P10" s="17"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="7"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="1"/>
+      <c r="L11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="11"/>
-      <c r="O11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="12"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="7"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="15" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="15"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="1"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="16"/>
+      <c r="P12" s="17"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="7"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="1"/>
+      <c r="B13" s="22"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="7"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="1"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="7"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="1"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="7"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="27" t="s">
+      <c r="K16" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="27" t="s">
+      <c r="L16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="28" t="s">
+      <c r="M16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="27" t="s">
+      <c r="N16" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="27" t="s">
+      <c r="O16" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="P16" s="27" t="s">
+      <c r="P16" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="27" t="s">
+      <c r="Q16" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="R16" s="29" t="s">
+      <c r="R16" s="26" t="s">
         <v>31</v>
+      </c>
+      <c r="S16" s="29" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="10" t="s">
-        <v>32</v>
+      <c r="B17" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="D17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="E17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="F17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="G17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="H17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="I17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="J17" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="K17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="M17" s="31" t="s">
+      <c r="L17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="M17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="O17" s="11" t="s">
+      <c r="N17" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="P17" s="11" t="s">
+      <c r="O17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="P17" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="32" t="s">
+      <c r="Q17" s="12" t="s">
         <v>48</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="S17" s="33" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
       <c r="R18" s="35"/>
+      <c r="S18" s="36"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1908,8 +1919,8 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B12:J13"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B12:K13"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Added Brand name in the partner invoice Annexure file #CRM-1391
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>ANNEXURE - INSTALLATION &amp; DEMO</t>
   </si>
@@ -79,6 +79,9 @@
     <t>Product</t>
   </si>
   <si>
+    <t>Brand</t>
+  </si>
+  <si>
     <t>Category</t>
   </si>
   <si>
@@ -131,6 +134,9 @@
   </si>
   <si>
     <t>{booking:services}</t>
+  </si>
+  <si>
+    <t>{booking:appliance_brand}</t>
   </si>
   <si>
     <t>{booking:appliance_category}</t>
@@ -465,14 +471,13 @@
     <col customWidth="1" min="2" max="2" width="14.14"/>
     <col customWidth="1" min="3" max="3" width="16.0"/>
     <col customWidth="1" min="4" max="6" width="18.57"/>
-    <col customWidth="1" min="7" max="9" width="14.14"/>
-    <col customWidth="1" min="10" max="10" width="19.57"/>
-    <col customWidth="1" min="11" max="11" width="14.14"/>
-    <col customWidth="1" min="12" max="13" width="23.0"/>
-    <col customWidth="1" min="14" max="15" width="18.43"/>
-    <col customWidth="1" min="16" max="16" width="21.71"/>
-    <col customWidth="1" min="17" max="19" width="14.14"/>
-    <col customWidth="1" min="20" max="27" width="8.71"/>
+    <col customWidth="1" min="7" max="10" width="14.14"/>
+    <col customWidth="1" min="11" max="11" width="19.57"/>
+    <col customWidth="1" min="12" max="12" width="14.14"/>
+    <col customWidth="1" min="13" max="14" width="23.0"/>
+    <col customWidth="1" min="15" max="16" width="18.43"/>
+    <col customWidth="1" min="17" max="17" width="21.71"/>
+    <col customWidth="1" min="18" max="20" width="14.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -494,6 +499,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -515,8 +521,9 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -537,7 +544,8 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
-      <c r="S3" s="7"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -560,7 +568,8 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
-      <c r="S4" s="7"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
@@ -576,15 +585,16 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="1"/>
+      <c r="M5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="12"/>
-      <c r="P5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="12"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="7"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -600,15 +610,16 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="1"/>
+      <c r="M6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="12"/>
-      <c r="P6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="12"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="7"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
@@ -624,15 +635,16 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="1"/>
+      <c r="M7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="12"/>
-      <c r="P7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="12"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="7"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -645,14 +657,15 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="13"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="O8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="7"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -665,14 +678,15 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="O9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="7"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
@@ -687,16 +701,17 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="16" t="s">
+      <c r="K10" s="13"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="16"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="16"/>
+      <c r="Q10" s="17"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="7"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
@@ -712,15 +727,16 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="1"/>
+      <c r="M11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="12"/>
-      <c r="P11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="12"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="7"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
@@ -736,27 +752,28 @@
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
-      <c r="L12" s="16" t="s">
+      <c r="L12" s="21"/>
+      <c r="M12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="17"/>
-      <c r="N12" s="16"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="1"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="16"/>
+      <c r="Q12" s="17"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="7"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="22"/>
-      <c r="L13" s="17"/>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="1"/>
+      <c r="Q13" s="17"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="7"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
@@ -777,9 +794,10 @@
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
-      <c r="Q14" s="1"/>
+      <c r="Q14" s="17"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="7"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
@@ -798,9 +816,10 @@
       <c r="N15" s="17"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="17"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="7"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
@@ -813,7 +832,7 @@
       <c r="D16" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="26" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="26" t="s">
@@ -825,7 +844,7 @@
       <c r="H16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="27" t="s">
         <v>22</v>
       </c>
       <c r="J16" s="26" t="s">
@@ -840,10 +859,10 @@
       <c r="M16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="28" t="s">
+      <c r="N16" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="26" t="s">
+      <c r="O16" s="28" t="s">
         <v>28</v>
       </c>
       <c r="P16" s="26" t="s">
@@ -855,65 +874,71 @@
       <c r="R16" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="S16" s="29" t="s">
+      <c r="S16" s="26" t="s">
         <v>32</v>
+      </c>
+      <c r="T16" s="29" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="31" t="s">
         <v>36</v>
       </c>
+      <c r="E17" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="12" t="s">
         <v>40</v>
       </c>
+      <c r="I17" s="31" t="s">
+        <v>41</v>
+      </c>
       <c r="J17" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="N17" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="12" t="s">
+      <c r="N17" s="12" t="s">
         <v>46</v>
       </c>
+      <c r="O17" s="32" t="s">
+        <v>47</v>
+      </c>
       <c r="P17" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="S17" s="33" t="s">
         <v>50</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="T17" s="33" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -935,7 +960,8 @@
       <c r="P18" s="35"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="35"/>
-      <c r="S18" s="36"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="36"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1919,8 +1945,8 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B12:K13"/>
+    <mergeCell ref="B12:L13"/>
+    <mergeCell ref="B2:R2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Download Model Number/SF Model No in the Invoice Annxure file #CRM-1425
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>ANNEXURE - INSTALLATION &amp; DEMO</t>
   </si>
@@ -88,6 +88,9 @@
     <t>Size</t>
   </si>
   <si>
+    <t>Model Number</t>
+  </si>
+  <si>
     <t>City</t>
   </si>
   <si>
@@ -143,6 +146,9 @@
   </si>
   <si>
     <t>{booking:appliance_capacity}</t>
+  </si>
+  <si>
+    <t>{booking:model_number}</t>
   </si>
   <si>
     <t>{booking:city}</t>
@@ -472,12 +478,12 @@
     <col customWidth="1" min="3" max="3" width="16.0"/>
     <col customWidth="1" min="4" max="6" width="18.57"/>
     <col customWidth="1" min="7" max="10" width="14.14"/>
-    <col customWidth="1" min="11" max="11" width="19.57"/>
-    <col customWidth="1" min="12" max="12" width="14.14"/>
-    <col customWidth="1" min="13" max="14" width="23.0"/>
-    <col customWidth="1" min="15" max="16" width="18.43"/>
-    <col customWidth="1" min="17" max="17" width="21.71"/>
-    <col customWidth="1" min="18" max="20" width="14.14"/>
+    <col customWidth="1" min="11" max="12" width="19.57"/>
+    <col customWidth="1" min="13" max="13" width="14.14"/>
+    <col customWidth="1" min="14" max="15" width="23.0"/>
+    <col customWidth="1" min="16" max="17" width="18.43"/>
+    <col customWidth="1" min="18" max="18" width="21.71"/>
+    <col customWidth="1" min="19" max="21" width="14.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -500,6 +506,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -522,8 +529,9 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="5"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -545,7 +553,8 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="7"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -569,7 +578,8 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="7"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
@@ -586,15 +596,16 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="1"/>
+      <c r="N5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="1"/>
-      <c r="O5" s="12"/>
-      <c r="Q5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="12"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="7"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -611,15 +622,16 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="1"/>
+      <c r="N6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="12"/>
-      <c r="Q6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="12"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="7"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
@@ -636,15 +648,16 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="1"/>
+      <c r="N7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="12"/>
-      <c r="Q7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="12"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="7"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -658,14 +671,15 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="P8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="7"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -679,14 +693,15 @@
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="13"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="P9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="7"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
@@ -702,16 +717,17 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="16" t="s">
+      <c r="L10" s="13"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="1"/>
-      <c r="O10" s="16"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="16"/>
+      <c r="R10" s="17"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="7"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
@@ -728,15 +744,16 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="12" t="s">
+      <c r="M11" s="1"/>
+      <c r="N11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="12"/>
-      <c r="Q11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="12"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="7"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
@@ -753,27 +770,28 @@
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="21"/>
+      <c r="N12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="17"/>
-      <c r="O12" s="16"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="1"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="16"/>
+      <c r="R12" s="17"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="7"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="22"/>
-      <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
-      <c r="R13" s="1"/>
+      <c r="R13" s="17"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="7"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
@@ -795,9 +813,10 @@
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="17"/>
-      <c r="R14" s="1"/>
+      <c r="R14" s="17"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="7"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
@@ -817,9 +836,10 @@
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
-      <c r="R15" s="1"/>
+      <c r="R15" s="17"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="7"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
@@ -844,7 +864,7 @@
       <c r="H16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="26" t="s">
         <v>22</v>
       </c>
       <c r="J16" s="26" t="s">
@@ -853,7 +873,7 @@
       <c r="K16" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="26" t="s">
+      <c r="L16" s="27" t="s">
         <v>25</v>
       </c>
       <c r="M16" s="26" t="s">
@@ -862,10 +882,10 @@
       <c r="N16" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="28" t="s">
+      <c r="O16" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="P16" s="26" t="s">
+      <c r="P16" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Q16" s="26" t="s">
@@ -877,68 +897,74 @@
       <c r="S16" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="T16" s="29" t="s">
+      <c r="T16" s="26" t="s">
         <v>33</v>
+      </c>
+      <c r="U16" s="29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="31" t="s">
         <v>41</v>
       </c>
+      <c r="I17" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="J17" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="L17" s="31" t="s">
+        <v>45</v>
+      </c>
       <c r="M17" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="O17" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="P17" s="12" t="s">
+      <c r="O17" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="P17" s="32" t="s">
+        <v>49</v>
+      </c>
       <c r="Q17" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R17" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S17" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="T17" s="33" t="s">
         <v>52</v>
+      </c>
+      <c r="T17" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="U17" s="33" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -961,7 +987,8 @@
       <c r="Q18" s="35"/>
       <c r="R18" s="35"/>
       <c r="S18" s="35"/>
-      <c r="T18" s="36"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="36"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1945,8 +1972,8 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B12:L13"/>
-    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B12:M13"/>
+    <mergeCell ref="B2:S2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Invoices Changes #CRM-1552  #CRM-1554 #CRM-1550 #CRM-1414
1.In Annexure add upcountry yes/No column. It makes easy for them for
analysis #CRM-1552
2.Update Invoice with invoice break up details #CRM-1554
3. Update Partner Invoice ID, Booking ID, paid charge in the courier
comapay invoice details Table #CRM-1550
3. Call Centre / Warehouse Charges for Partners in Monthly Invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>ANNEXURE - INSTALLATION &amp; DEMO</t>
   </si>
@@ -94,6 +94,9 @@
     <t>City</t>
   </si>
   <si>
+    <t>Upcountry</t>
+  </si>
+  <si>
     <t>Booking ID</t>
   </si>
   <si>
@@ -152,6 +155,9 @@
   </si>
   <si>
     <t>{booking:city}</t>
+  </si>
+  <si>
+    <t>{booking:upcountry}</t>
   </si>
   <si>
     <t>{booking:booking_id}</t>
@@ -345,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -408,6 +414,9 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -479,11 +488,11 @@
     <col customWidth="1" min="4" max="6" width="18.57"/>
     <col customWidth="1" min="7" max="10" width="14.14"/>
     <col customWidth="1" min="11" max="12" width="19.57"/>
-    <col customWidth="1" min="13" max="13" width="14.14"/>
-    <col customWidth="1" min="14" max="15" width="23.0"/>
-    <col customWidth="1" min="16" max="17" width="18.43"/>
-    <col customWidth="1" min="18" max="18" width="21.71"/>
-    <col customWidth="1" min="19" max="21" width="14.14"/>
+    <col customWidth="1" min="13" max="14" width="14.14"/>
+    <col customWidth="1" min="15" max="16" width="23.0"/>
+    <col customWidth="1" min="17" max="18" width="18.43"/>
+    <col customWidth="1" min="19" max="19" width="21.71"/>
+    <col customWidth="1" min="20" max="22" width="14.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -507,6 +516,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -530,8 +540,9 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="5"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -554,7 +565,8 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="U3" s="7"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -579,7 +591,8 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="7"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
@@ -597,15 +610,16 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="1"/>
+      <c r="O5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="12"/>
-      <c r="R5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="12"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="7"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -623,15 +637,16 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="1"/>
+      <c r="O6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="12"/>
-      <c r="R6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="12"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="7"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
@@ -649,15 +664,16 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="1"/>
+      <c r="O7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="12"/>
-      <c r="R7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="12"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="7"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -676,10 +692,11 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="Q8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="7"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -698,10 +715,11 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="Q9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="7"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
@@ -719,15 +737,16 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="16" t="s">
+      <c r="N10" s="1"/>
+      <c r="O10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="16"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="16"/>
+      <c r="S10" s="17"/>
       <c r="T10" s="1"/>
-      <c r="U10" s="7"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
@@ -745,15 +764,16 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="12" t="s">
+      <c r="N11" s="1"/>
+      <c r="O11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="12"/>
-      <c r="R11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="12"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
-      <c r="U11" s="7"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
@@ -771,27 +791,29 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
-      <c r="N12" s="16" t="s">
+      <c r="N12" s="22"/>
+      <c r="O12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="O12" s="17"/>
-      <c r="P12" s="16"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="1"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="16"/>
+      <c r="S12" s="17"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="7"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="22"/>
-      <c r="N13" s="17"/>
+      <c r="B13" s="23"/>
+      <c r="N13" s="22"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
-      <c r="S13" s="1"/>
+      <c r="S13" s="17"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="7"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
@@ -814,13 +836,14 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
-      <c r="S14" s="1"/>
+      <c r="S14" s="17"/>
       <c r="T14" s="1"/>
-      <c r="U14" s="7"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -837,158 +860,166 @@
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
-      <c r="S15" s="1"/>
+      <c r="S15" s="17"/>
       <c r="T15" s="1"/>
-      <c r="U15" s="7"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="27" t="s">
         <v>24</v>
       </c>
       <c r="L16" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="26" t="s">
+      <c r="M16" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="26" t="s">
+      <c r="N16" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="26" t="s">
+      <c r="O16" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P16" s="28" t="s">
+      <c r="P16" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="26" t="s">
+      <c r="Q16" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="R16" s="26" t="s">
+      <c r="R16" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="S16" s="26" t="s">
+      <c r="S16" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="T16" s="26" t="s">
+      <c r="T16" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="29" t="s">
+      <c r="U16" s="27" t="s">
         <v>34</v>
+      </c>
+      <c r="V16" s="30" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="30" t="s">
         <v>36</v>
       </c>
+      <c r="C17" s="31" t="s">
+        <v>37</v>
+      </c>
       <c r="D17" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="L17" s="31" t="s">
         <v>45</v>
       </c>
+      <c r="L17" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="M17" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="N17" s="12" t="s">
         <v>47</v>
       </c>
+      <c r="N17" s="32" t="s">
+        <v>48</v>
+      </c>
       <c r="O17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="P17" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="Q17" s="12" t="s">
+      <c r="P17" s="12" t="s">
         <v>50</v>
       </c>
+      <c r="Q17" s="33" t="s">
+        <v>51</v>
+      </c>
       <c r="R17" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S17" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="U17" s="33" t="s">
         <v>54</v>
+      </c>
+      <c r="U17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V17" s="34" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
       <c r="U18" s="36"/>
+      <c r="V18" s="37"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1973,7 +2004,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B12:M13"/>
-    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B2:T2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Remove Dash( - ) From Paytm Annxure Invoice & Add Order Support file link in the Partner Invoice Annxure #CRM-1638 #CRM-1645
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>ANNEXURE - INSTALLATION &amp; DEMO</t>
   </si>
@@ -121,6 +121,9 @@
     <t>GST Amount</t>
   </si>
   <si>
+    <t>Order Support File</t>
+  </si>
+  <si>
     <t>{booking:order_id}</t>
   </si>
   <si>
@@ -182,6 +185,9 @@
   </si>
   <si>
     <t>{booking:gst_amount}</t>
+  </si>
+  <si>
+    <t>{booking:support_file}</t>
   </si>
 </sst>
 </file>
@@ -430,26 +436,26 @@
     <xf borderId="7" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="7" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="10" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -492,7 +498,7 @@
     <col customWidth="1" min="15" max="16" width="23.0"/>
     <col customWidth="1" min="17" max="18" width="18.43"/>
     <col customWidth="1" min="19" max="19" width="21.71"/>
-    <col customWidth="1" min="20" max="22" width="14.14"/>
+    <col customWidth="1" min="20" max="23" width="14.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -517,6 +523,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -542,7 +549,8 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="4"/>
-      <c r="V2" s="5"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -566,7 +574,8 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
-      <c r="V3" s="7"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -592,7 +601,8 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="7"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
@@ -619,7 +629,8 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="7"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -646,7 +657,8 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="7"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
@@ -673,7 +685,8 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="7"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -696,7 +709,8 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="7"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -719,7 +733,8 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="7"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
@@ -746,7 +761,8 @@
       <c r="S10" s="17"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="7"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
@@ -773,7 +789,8 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="7"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
@@ -800,7 +817,8 @@
       <c r="S12" s="17"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="7"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
@@ -813,7 +831,8 @@
       <c r="S13" s="17"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
-      <c r="V13" s="7"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
@@ -839,7 +858,8 @@
       <c r="S14" s="17"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="7"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
@@ -863,7 +883,8 @@
       <c r="S15" s="17"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-      <c r="V15" s="7"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
@@ -903,7 +924,7 @@
       <c r="M16" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="28" t="s">
+      <c r="N16" s="27" t="s">
         <v>27</v>
       </c>
       <c r="O16" s="27" t="s">
@@ -912,7 +933,7 @@
       <c r="P16" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="29" t="s">
+      <c r="Q16" s="28" t="s">
         <v>30</v>
       </c>
       <c r="R16" s="27" t="s">
@@ -927,74 +948,80 @@
       <c r="U16" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="V16" s="30" t="s">
+      <c r="V16" s="29" t="s">
         <v>35</v>
+      </c>
+      <c r="W16" s="30" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="N17" s="32" t="s">
         <v>48</v>
       </c>
+      <c r="N17" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="O17" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q17" s="33" t="s">
         <v>51</v>
       </c>
+      <c r="Q17" s="32" t="s">
+        <v>52</v>
+      </c>
       <c r="R17" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S17" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="U17" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V17" s="34" t="s">
         <v>56</v>
+      </c>
+      <c r="V17" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="W17" s="34" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -1019,7 +1046,8 @@
       <c r="S18" s="36"/>
       <c r="T18" s="36"/>
       <c r="U18" s="36"/>
-      <c r="V18" s="37"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="37"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
CRM-3851 : Invoice annexure format issues
1. sub-order id format should be corrected, coming as exponential
2. same for item order id
3. courier <= 1 should not go
4. same for upcountry, upcountry price <= 1 should not go
5. image links should come in the last column
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -82,9 +82,6 @@
     <t>Serial Number</t>
   </si>
   <si>
-    <t>Serial Number Imag</t>
-  </si>
-  <si>
     <t>Customer Name</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
     <t>GST Amount</t>
   </si>
   <si>
+    <t>Serial Number Image</t>
+  </si>
+  <si>
     <t>Order Support File</t>
   </si>
   <si>
@@ -151,61 +151,61 @@
     <t>{booking:serial_number}</t>
   </si>
   <si>
+    <t>{booking:name}</t>
+  </si>
+  <si>
+    <t>{booking:booking_primary_contact_no}</t>
+  </si>
+  <si>
+    <t>{booking:services}</t>
+  </si>
+  <si>
+    <t>{booking:appliance_brand}</t>
+  </si>
+  <si>
+    <t>{booking:appliance_category}</t>
+  </si>
+  <si>
+    <t>{booking:appliance_capacity}</t>
+  </si>
+  <si>
+    <t>{booking:model_number}</t>
+  </si>
+  <si>
+    <t>{booking:city}</t>
+  </si>
+  <si>
+    <t>{booking:state}</t>
+  </si>
+  <si>
+    <t>{booking:upcountry}</t>
+  </si>
+  <si>
+    <t>{booking:booking_id}</t>
+  </si>
+  <si>
+    <t>{booking:unit_id}</t>
+  </si>
+  <si>
+    <t>{booking:booking_date}</t>
+  </si>
+  <si>
+    <t>{booking:closed_date}</t>
+  </si>
+  <si>
+    <t>{booking:price_tags}</t>
+  </si>
+  <si>
+    <t>{booking:rating_stars}</t>
+  </si>
+  <si>
+    <t>{booking:partner_net_payable}</t>
+  </si>
+  <si>
+    <t>{booking:gst_amount}</t>
+  </si>
+  <si>
     <t>{booking:serial_number_pic}</t>
-  </si>
-  <si>
-    <t>{booking:name}</t>
-  </si>
-  <si>
-    <t>{booking:booking_primary_contact_no}</t>
-  </si>
-  <si>
-    <t>{booking:services}</t>
-  </si>
-  <si>
-    <t>{booking:appliance_brand}</t>
-  </si>
-  <si>
-    <t>{booking:appliance_category}</t>
-  </si>
-  <si>
-    <t>{booking:appliance_capacity}</t>
-  </si>
-  <si>
-    <t>{booking:model_number}</t>
-  </si>
-  <si>
-    <t>{booking:city}</t>
-  </si>
-  <si>
-    <t>{booking:state}</t>
-  </si>
-  <si>
-    <t>{booking:upcountry}</t>
-  </si>
-  <si>
-    <t>{booking:booking_id}</t>
-  </si>
-  <si>
-    <t>{booking:unit_id}</t>
-  </si>
-  <si>
-    <t>{booking:booking_date}</t>
-  </si>
-  <si>
-    <t>{booking:closed_date}</t>
-  </si>
-  <si>
-    <t>{booking:price_tags}</t>
-  </si>
-  <si>
-    <t>{booking:rating_stars}</t>
-  </si>
-  <si>
-    <t>{booking:partner_net_payable}</t>
-  </si>
-  <si>
-    <t>{booking:gst_amount}</t>
   </si>
   <si>
     <t>{booking:support_file}</t>
@@ -215,7 +215,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -253,11 +253,6 @@
       <b/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
@@ -365,12 +360,8 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left style="medium">
@@ -397,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -458,7 +449,7 @@
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -470,23 +461,14 @@
     <xf borderId="6" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="6" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="14" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -726,7 +708,9 @@
     <col customWidth="1" min="16" max="17" width="23.0"/>
     <col customWidth="1" min="18" max="19" width="18.43"/>
     <col customWidth="1" min="20" max="20" width="21.71"/>
-    <col customWidth="1" min="21" max="24" width="14.14"/>
+    <col customWidth="1" min="21" max="22" width="14.14"/>
+    <col customWidth="1" min="23" max="23" width="22.29"/>
+    <col customWidth="1" min="24" max="24" width="20.29"/>
     <col customWidth="1" min="25" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -1188,10 +1172,10 @@
       <c r="P16" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="29" t="s">
+      <c r="Q16" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="R16" s="30" t="s">
+      <c r="R16" s="29" t="s">
         <v>31</v>
       </c>
       <c r="S16" s="29" t="s">
@@ -1206,10 +1190,10 @@
       <c r="V16" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="W16" s="31" t="s">
+      <c r="W16" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="X16" s="31" t="s">
+      <c r="X16" s="30" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1218,7 +1202,7 @@
       <c r="B17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="22" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -1260,10 +1244,10 @@
       <c r="P17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="Q17" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="R17" s="33" t="s">
+      <c r="R17" s="11" t="s">
         <v>54</v>
       </c>
       <c r="S17" s="11" t="s">
@@ -1278,38 +1262,38 @@
       <c r="V17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="W17" s="34" t="s">
+      <c r="W17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="X17" s="34" t="s">
+      <c r="X17" s="31" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="37"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="34"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Attach Spare extra charges in the Partner Main Invoice #CRMS-627
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>ANNEXURE - INSTALLATION &amp; DEMO</t>
   </si>
@@ -127,6 +127,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Spare Involved</t>
+  </si>
+  <si>
     <t>Rating</t>
   </si>
   <si>
@@ -194,6 +197,9 @@
   </si>
   <si>
     <t>{booking:price_tags}</t>
+  </si>
+  <si>
+    <t>{booking:spare_involved}</t>
   </si>
   <si>
     <t>{booking:rating_stars}</t>
@@ -282,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="14">
     <border/>
     <border>
       <left style="medium">
@@ -339,23 +345,6 @@
       <top/>
     </border>
     <border>
-      <right/>
-      <top/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <bottom/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -388,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -448,13 +437,10 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -467,19 +453,25 @@
     <xf borderId="7" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -706,12 +698,11 @@
     <col customWidth="1" min="11" max="12" width="19.57"/>
     <col customWidth="1" min="13" max="15" width="14.14"/>
     <col customWidth="1" min="16" max="17" width="23.0"/>
-    <col customWidth="1" min="18" max="19" width="18.43"/>
-    <col customWidth="1" min="20" max="20" width="21.71"/>
-    <col customWidth="1" min="21" max="22" width="14.14"/>
-    <col customWidth="1" min="23" max="23" width="22.29"/>
-    <col customWidth="1" min="24" max="24" width="20.29"/>
-    <col customWidth="1" min="25" max="26" width="8.71"/>
+    <col customWidth="1" min="18" max="20" width="18.43"/>
+    <col customWidth="1" min="21" max="21" width="21.71"/>
+    <col customWidth="1" min="22" max="23" width="14.14"/>
+    <col customWidth="1" min="24" max="24" width="22.29"/>
+    <col customWidth="1" min="25" max="25" width="20.29"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -738,6 +729,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -763,9 +755,10 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
-      <c r="V2" s="4"/>
+      <c r="V2" s="3"/>
       <c r="W2" s="4"/>
-      <c r="X2" s="5"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -791,7 +784,8 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="7"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -819,7 +813,8 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="7"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
@@ -844,11 +839,11 @@
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="11"/>
-      <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="7"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -873,11 +868,11 @@
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="11"/>
-      <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
-      <c r="X6" s="7"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
@@ -902,11 +897,11 @@
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="11"/>
-      <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
-      <c r="X7" s="7"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -927,11 +922,11 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="7"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -952,11 +947,11 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
-      <c r="X9" s="7"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
@@ -981,11 +976,11 @@
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="16"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="1"/>
+      <c r="U10" s="17"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="7"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
@@ -1010,11 +1005,11 @@
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="11"/>
-      <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
-      <c r="X11" s="7"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
@@ -1031,45 +1026,35 @@
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="22"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="21"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="17"/>
       <c r="R12" s="16"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="1"/>
+      <c r="U12" s="17"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="7"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="N13" s="21"/>
       <c r="O13" s="16"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
-      <c r="U13" s="1"/>
+      <c r="U13" s="17"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
-      <c r="X13" s="7"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
@@ -1094,14 +1079,15 @@
       <c r="R14" s="17"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
-      <c r="U14" s="1"/>
+      <c r="U14" s="17"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="7"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="26"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -1120,180 +1106,188 @@
       <c r="R15" s="17"/>
       <c r="S15" s="17"/>
       <c r="T15" s="17"/>
-      <c r="U15" s="1"/>
+      <c r="U15" s="17"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
-      <c r="X15" s="7"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="29" t="s">
+      <c r="L16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="29" t="s">
+      <c r="M16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="29" t="s">
+      <c r="N16" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="29" t="s">
+      <c r="O16" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="P16" s="29" t="s">
+      <c r="P16" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="28" t="s">
+      <c r="Q16" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="R16" s="29" t="s">
+      <c r="R16" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="S16" s="29" t="s">
+      <c r="S16" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="T16" s="29" t="s">
+      <c r="T16" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="29" t="s">
+      <c r="U16" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="V16" s="29" t="s">
+      <c r="V16" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="W16" s="29" t="s">
+      <c r="W16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="X16" s="30" t="s">
+      <c r="X16" s="26" t="s">
         <v>37</v>
+      </c>
+      <c r="Y16" s="28" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="22" t="s">
         <v>39</v>
       </c>
+      <c r="C17" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="D17" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q17" s="22" t="s">
         <v>53</v>
       </c>
+      <c r="Q17" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="R17" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="T17" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="T17" s="29" t="s">
+        <v>57</v>
+      </c>
       <c r="U17" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W17" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="X17" s="31" t="s">
         <v>60</v>
+      </c>
+      <c r="X17" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y17" s="30" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="33"/>
-      <c r="V18" s="33"/>
-      <c r="W18" s="33"/>
-      <c r="X18" s="34"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="33"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -2277,8 +2271,8 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:U2"/>
     <mergeCell ref="B12:M13"/>
+    <mergeCell ref="B2:V2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Sf closed date added in invoice annx file #CRMS-1468
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>ANNEXURE - INSTALLATION &amp; DEMO</t>
   </si>
@@ -124,6 +124,9 @@
     <t>Closed Date</t>
   </si>
   <si>
+    <t>Sf Closed Date</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
@@ -194,6 +197,9 @@
   </si>
   <si>
     <t>{booking:closed_date}</t>
+  </si>
+  <si>
+    <t>{booking:service_center_closed_date}</t>
   </si>
   <si>
     <t>{booking:price_tags}</t>
@@ -377,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -425,6 +431,9 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -698,11 +707,11 @@
     <col customWidth="1" min="11" max="12" width="19.57"/>
     <col customWidth="1" min="13" max="15" width="14.14"/>
     <col customWidth="1" min="16" max="17" width="23.0"/>
-    <col customWidth="1" min="18" max="20" width="18.43"/>
-    <col customWidth="1" min="21" max="21" width="21.71"/>
-    <col customWidth="1" min="22" max="23" width="14.14"/>
-    <col customWidth="1" min="24" max="24" width="22.29"/>
-    <col customWidth="1" min="25" max="25" width="20.29"/>
+    <col customWidth="1" min="18" max="21" width="18.43"/>
+    <col customWidth="1" min="22" max="22" width="21.71"/>
+    <col customWidth="1" min="23" max="24" width="14.14"/>
+    <col customWidth="1" min="25" max="25" width="22.29"/>
+    <col customWidth="1" min="26" max="26" width="20.29"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -730,6 +739,7 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -756,9 +766,10 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
-      <c r="W2" s="4"/>
+      <c r="W2" s="3"/>
       <c r="X2" s="4"/>
-      <c r="Y2" s="5"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -785,7 +796,8 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Y3" s="7"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -814,7 +826,8 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="7"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
@@ -839,11 +852,12 @@
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="11"/>
-      <c r="U5" s="1"/>
+      <c r="S5" s="11"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="7"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -868,11 +882,12 @@
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="11"/>
-      <c r="U6" s="1"/>
+      <c r="S6" s="11"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="7"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
@@ -897,11 +912,12 @@
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="11"/>
-      <c r="U7" s="1"/>
+      <c r="S7" s="11"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
-      <c r="Y7" s="7"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -922,11 +938,12 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="U8" s="1"/>
+      <c r="S8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
-      <c r="Y8" s="7"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -947,11 +964,12 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="U9" s="1"/>
+      <c r="S9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-      <c r="Y9" s="7"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
@@ -976,15 +994,16 @@
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="16"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="1"/>
+      <c r="S10" s="17"/>
+      <c r="V10" s="18"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Y10" s="7"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="16"/>
@@ -1005,289 +1024,301 @@
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="11"/>
-      <c r="U11" s="1"/>
+      <c r="S11" s="11"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="7"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="17"/>
+      <c r="Q12" s="18"/>
       <c r="R12" s="16"/>
-      <c r="U12" s="17"/>
-      <c r="V12" s="1"/>
+      <c r="S12" s="17"/>
+      <c r="V12" s="18"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="7"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="22"/>
-      <c r="N13" s="21"/>
+      <c r="B13" s="23"/>
+      <c r="N13" s="22"/>
       <c r="O13" s="16"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="1"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-      <c r="Y13" s="7"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="1"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-      <c r="Y14" s="7"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="1"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
-      <c r="Y15" s="7"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="26" t="s">
+      <c r="L16" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="26" t="s">
+      <c r="M16" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="26" t="s">
+      <c r="N16" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="26" t="s">
+      <c r="O16" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P16" s="26" t="s">
+      <c r="P16" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="25" t="s">
+      <c r="Q16" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="R16" s="26" t="s">
+      <c r="R16" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="S16" s="26" t="s">
+      <c r="S16" s="28" t="s">
         <v>32</v>
       </c>
       <c r="T16" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="26" t="s">
+      <c r="U16" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="V16" s="26" t="s">
+      <c r="V16" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="W16" s="26" t="s">
+      <c r="W16" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="X16" s="26" t="s">
+      <c r="X16" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="Y16" s="28" t="s">
+      <c r="Y16" s="27" t="s">
         <v>38</v>
+      </c>
+      <c r="Z16" s="29" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="21" t="s">
         <v>40</v>
       </c>
+      <c r="C17" s="22" t="s">
+        <v>41</v>
+      </c>
       <c r="D17" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q17" s="21" t="s">
         <v>54</v>
       </c>
+      <c r="Q17" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="R17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="S17" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="T17" s="29" t="s">
+      <c r="S17" s="30" t="s">
         <v>57</v>
       </c>
+      <c r="T17" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="U17" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="W17" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="X17" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y17" s="30" t="s">
         <v>62</v>
+      </c>
+      <c r="Y17" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z17" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="32"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
       <c r="Y18" s="33"/>
+      <c r="Z18" s="34"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -2272,7 +2303,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B12:M13"/>
-    <mergeCell ref="B2:V2"/>
+    <mergeCell ref="B2:W2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>